<commit_message>
Update comment in the overlay dome file
1. SLRGF = Root distribution factor (documentation in each field overlay
spreadsheet)
2. Paddy management function -> remove “not yet functional” from
documentation in field overlay spreadsheets
</commit_message>
<xml_diff>
--- a/Maize_Machakos/raw/Field_Overlay.xlsx
+++ b/Maize_Machakos/raw/Field_Overlay.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-30" windowWidth="12495" windowHeight="11760"/>
+    <workbookView xWindow="12" yWindow="-36" windowWidth="12492" windowHeight="11556"/>
   </bookViews>
   <sheets>
     <sheet name="Field_Overlay" sheetId="6" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="171">
   <si>
     <t>cm</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>! Blank for survey simulation</t>
+  </si>
+  <si>
+    <t>Root distribution factor</t>
   </si>
 </sst>
 </file>
@@ -992,26 +995,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:D44"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="24" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
     <col min="11" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25">
+    <row r="1" spans="1:6" ht="16.8">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1143,7 +1144,7 @@
       <c r="C9"/>
       <c r="D9"/>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="17.25">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="16.8">
       <c r="A10" s="20" t="s">
         <v>1</v>
       </c>
@@ -1153,7 +1154,7 @@
       <c r="C10" s="23"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="30">
+    <row r="11" spans="1:6">
       <c r="A11" s="17" t="s">
         <v>1</v>
       </c>
@@ -1214,7 +1215,7 @@
       <c r="A15"/>
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:6" ht="17.25">
+    <row r="16" spans="1:6" ht="16.8">
       <c r="A16" s="20" t="s">
         <v>1</v>
       </c>
@@ -1225,7 +1226,7 @@
       <c r="D16" s="25"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" ht="30">
+    <row r="17" spans="1:9" s="1" customFormat="1">
       <c r="A17" s="19" t="s">
         <v>1</v>
       </c>
@@ -1242,7 +1243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30">
+    <row r="18" spans="1:9" ht="28.8">
       <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
@@ -1323,7 +1324,7 @@
     <row r="24" spans="1:9">
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:9" ht="60">
+    <row r="25" spans="1:9" ht="57.6">
       <c r="A25" s="10" t="s">
         <v>1</v>
       </c>
@@ -1458,7 +1459,7 @@
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:9" ht="17.25">
+    <row r="38" spans="1:9" ht="16.8">
       <c r="A38" s="20" t="s">
         <v>1</v>
       </c>
@@ -1468,7 +1469,7 @@
       <c r="C38" s="23"/>
       <c r="D38" s="22"/>
     </row>
-    <row r="39" spans="1:9" s="1" customFormat="1" ht="30">
+    <row r="39" spans="1:9" s="1" customFormat="1">
       <c r="A39" s="17" t="s">
         <v>1</v>
       </c>
@@ -1488,7 +1489,7 @@
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:9" ht="45">
+    <row r="40" spans="1:9" ht="43.2">
       <c r="A40" s="10" t="s">
         <v>1</v>
       </c>
@@ -1636,7 +1637,7 @@
       <c r="L50" s="33"/>
       <c r="M50" s="33"/>
     </row>
-    <row r="51" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="51" spans="1:13" s="1" customFormat="1" ht="28.8">
       <c r="A51" s="10" t="s">
         <v>1</v>
       </c>
@@ -1778,7 +1779,7 @@
       <c r="B62"/>
       <c r="D62"/>
     </row>
-    <row r="64" spans="1:13" ht="17.25">
+    <row r="64" spans="1:13" ht="16.8">
       <c r="A64" s="20" t="s">
         <v>1</v>
       </c>
@@ -1788,7 +1789,7 @@
       <c r="C64" s="23"/>
       <c r="D64" s="22"/>
     </row>
-    <row r="65" spans="1:14" ht="30">
+    <row r="65" spans="1:14">
       <c r="A65" s="17" t="s">
         <v>1</v>
       </c>
@@ -1812,7 +1813,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:14" s="5" customFormat="1" ht="90">
+    <row r="66" spans="1:14" s="5" customFormat="1" ht="72">
       <c r="A66" s="9" t="s">
         <v>1</v>
       </c>
@@ -1898,7 +1899,7 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:14" ht="17.25">
+    <row r="70" spans="1:14" ht="16.8">
       <c r="A70" s="20" t="s">
         <v>1</v>
       </c>
@@ -1908,7 +1909,7 @@
       <c r="C70" s="23"/>
       <c r="D70" s="22"/>
     </row>
-    <row r="71" spans="1:14" ht="30">
+    <row r="71" spans="1:14">
       <c r="A71" s="17" t="s">
         <v>1</v>
       </c>
@@ -1932,7 +1933,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:14" s="5" customFormat="1" ht="75">
+    <row r="72" spans="1:14" s="5" customFormat="1" ht="57.6">
       <c r="A72" s="9" t="s">
         <v>1</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="17.25">
+    <row r="76" spans="1:14" ht="16.8">
       <c r="A76" s="20" t="s">
         <v>1</v>
       </c>
@@ -2013,7 +2014,7 @@
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
     </row>
-    <row r="77" spans="1:14" s="1" customFormat="1" ht="30">
+    <row r="77" spans="1:14" s="1" customFormat="1">
       <c r="A77" s="19" t="s">
         <v>1</v>
       </c>
@@ -2034,13 +2035,13 @@
       <c r="M77"/>
       <c r="N77"/>
     </row>
-    <row r="78" spans="1:14" ht="60">
+    <row r="78" spans="1:14" ht="57.6">
       <c r="A78" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="9" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>55</v>
@@ -2078,7 +2079,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="60">
+    <row r="81" spans="1:8" ht="57.6">
       <c r="A81" s="10" t="s">
         <v>1</v>
       </c>
@@ -2125,7 +2126,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="60">
+    <row r="84" spans="1:8" ht="43.2">
       <c r="A84" s="10" t="s">
         <v>1</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="30">
+    <row r="90" spans="1:8" ht="28.8">
       <c r="A90" s="10" t="s">
         <v>1</v>
       </c>
@@ -2246,7 +2247,7 @@
     <row r="92" spans="1:8">
       <c r="B92"/>
     </row>
-    <row r="93" spans="1:8" ht="17.25">
+    <row r="93" spans="1:8" ht="16.8">
       <c r="A93" s="20" t="s">
         <v>1</v>
       </c>
@@ -2258,7 +2259,7 @@
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="94" spans="1:8" s="1" customFormat="1">
       <c r="A94" s="17" t="s">
         <v>1</v>
       </c>
@@ -2276,7 +2277,7 @@
       </c>
       <c r="F94" s="17"/>
     </row>
-    <row r="95" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="95" spans="1:8" s="1" customFormat="1">
       <c r="A95" s="10" t="s">
         <v>1</v>
       </c>
@@ -2319,7 +2320,7 @@
       <c r="B97" s="5"/>
       <c r="D97"/>
     </row>
-    <row r="98" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="98" spans="1:8" s="1" customFormat="1" ht="28.8">
       <c r="A98" s="10" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update overlay file for Machakos data set
Add APSIM soil parameters
</commit_message>
<xml_diff>
--- a/Maize_Machakos/raw/Field_Overlay.xlsx
+++ b/Maize_Machakos/raw/Field_Overlay.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="195">
   <si>
     <t>cm</t>
   </si>
@@ -527,6 +527,78 @@
   </si>
   <si>
     <t>Root distribution factor</t>
+  </si>
+  <si>
+    <t>Soil water content, air dry</t>
+  </si>
+  <si>
+    <t>Soil water, lower limit</t>
+  </si>
+  <si>
+    <t>SLADR</t>
+  </si>
+  <si>
+    <t>$SLLL</t>
+  </si>
+  <si>
+    <t>APSIM Evaporative diffusion constant</t>
+  </si>
+  <si>
+    <t>DiffusConst</t>
+  </si>
+  <si>
+    <t>APSIM Evaporative diffusion slope</t>
+  </si>
+  <si>
+    <t>DiffusSlope</t>
+  </si>
+  <si>
+    <t>Apsim Cona soil evaporation</t>
+  </si>
+  <si>
+    <t>CONA</t>
+  </si>
+  <si>
+    <t>Summer soil evaporation, upper limit for stage 1</t>
+  </si>
+  <si>
+    <t>SummerU</t>
+  </si>
+  <si>
+    <t>Winter soil evaporation, upper limit for stage 1</t>
+  </si>
+  <si>
+    <t>WinterU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date to switch to SummerU </t>
+  </si>
+  <si>
+    <t>SummerDate__soil</t>
+  </si>
+  <si>
+    <t>03-21</t>
+  </si>
+  <si>
+    <t>Date to switch to WinterU</t>
+  </si>
+  <si>
+    <t>WinterDate__soil</t>
+  </si>
+  <si>
+    <t>09-21</t>
+  </si>
+  <si>
+    <t>APSIM plant specific water uptake coefficient</t>
+  </si>
+  <si>
+    <t>apsim_kl</t>
+  </si>
+  <si>
+    <t>Biologically active soil organic carbon by layer</t>
+  </si>
+  <si>
+    <t>slacc</t>
   </si>
 </sst>
 </file>
@@ -611,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -693,6 +765,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,7 +1077,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N102"/>
+  <dimension ref="A1:N132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
@@ -2246,149 +2330,543 @@
     </row>
     <row r="92" spans="1:8">
       <c r="B92"/>
-    </row>
-    <row r="93" spans="1:8" ht="16.8">
-      <c r="A93" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B93" s="21" t="s">
+      <c r="D92" s="28"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:8" ht="28.8">
+      <c r="A93" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="10"/>
+      <c r="C93" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E93" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="F93" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E94" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F94" s="42">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="24"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:8" ht="28.8">
+      <c r="A96" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D96" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E96" s="36"/>
+      <c r="F96" s="36"/>
+      <c r="H96" s="32"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D97" s="28">
+        <v>40</v>
+      </c>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="24"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:8" ht="28.8">
+      <c r="A99" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" s="10"/>
+      <c r="C99" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D99" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E99" s="36"/>
+      <c r="F99" s="36"/>
+      <c r="H99" s="32"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="D100" s="28">
+        <v>16</v>
+      </c>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="24"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:8" ht="28.8">
+      <c r="A102" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B102" s="10"/>
+      <c r="C102" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D102" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E102" s="36"/>
+      <c r="F102" s="36"/>
+      <c r="H102" s="32"/>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D103" s="28">
+        <v>3.5</v>
+      </c>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="24"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+    </row>
+    <row r="105" spans="1:8" ht="43.2">
+      <c r="A105" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="10"/>
+      <c r="C105" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D105" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E105" s="36"/>
+      <c r="F105" s="36"/>
+      <c r="H105" s="32"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="D106" s="28">
+        <v>6</v>
+      </c>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="24"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+    </row>
+    <row r="108" spans="1:8" ht="39" customHeight="1">
+      <c r="A108" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" s="10"/>
+      <c r="C108" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D108" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E108" s="36"/>
+      <c r="F108" s="36"/>
+      <c r="H108" s="32"/>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D109" s="28">
+        <v>6</v>
+      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="24"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+    </row>
+    <row r="111" spans="1:8" ht="28.8">
+      <c r="A111" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" s="10"/>
+      <c r="C111" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D111" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E111" s="36"/>
+      <c r="F111" s="36"/>
+      <c r="H111" s="32"/>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C112" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D112" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="24"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+    </row>
+    <row r="114" spans="1:8" ht="39" customHeight="1">
+      <c r="A114" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="10"/>
+      <c r="C114" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D114" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E114" s="36"/>
+      <c r="F114" s="36"/>
+      <c r="H114" s="32"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="D115" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="24"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+    </row>
+    <row r="117" spans="1:8" ht="43.2">
+      <c r="A117" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B117" s="10"/>
+      <c r="C117" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D117" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E117" s="36"/>
+      <c r="F117" s="36"/>
+      <c r="H117" s="32"/>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D118" s="28">
+        <v>0.06</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="24"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+    </row>
+    <row r="120" spans="1:8" ht="28.8">
+      <c r="A120" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="10"/>
+      <c r="C120" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D120" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E120" s="36"/>
+      <c r="F120" s="36"/>
+      <c r="H120" s="32"/>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="D121" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="B122"/>
+    </row>
+    <row r="123" spans="1:8" ht="16.8">
+      <c r="A123" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B123" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C93" s="22"/>
-      <c r="D93" s="22"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:8" s="1" customFormat="1">
-      <c r="A94" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B94" s="18" t="s">
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+    </row>
+    <row r="124" spans="1:8" s="1" customFormat="1">
+      <c r="A124" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B124" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C94" s="18" t="s">
+      <c r="C124" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D94" s="17" t="s">
+      <c r="D124" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E94" s="17" t="s">
+      <c r="E124" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F94" s="17"/>
-    </row>
-    <row r="95" spans="1:8" s="1" customFormat="1">
-      <c r="A95" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B95" s="9"/>
-      <c r="C95" s="9" t="s">
+      <c r="F124" s="17"/>
+    </row>
+    <row r="125" spans="1:8" s="1" customFormat="1">
+      <c r="A125" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B125" s="9"/>
+      <c r="C125" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10" t="s">
+      <c r="D125" s="10"/>
+      <c r="E125" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F95" s="10" t="s">
+      <c r="F125" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H125" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C96" s="5" t="s">
+    <row r="126" spans="1:8">
+      <c r="A126" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D126" t="s">
         <v>110</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E126" t="s">
         <v>37</v>
       </c>
-      <c r="F96">
+      <c r="F126">
         <v>-30</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
-      <c r="B97" s="5"/>
-      <c r="D97"/>
-    </row>
-    <row r="98" spans="1:8" s="1" customFormat="1" ht="28.8">
-      <c r="A98" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B98" s="10"/>
-      <c r="C98" s="9" t="s">
+    <row r="127" spans="1:8">
+      <c r="B127" s="5"/>
+      <c r="D127"/>
+    </row>
+    <row r="128" spans="1:8" s="1" customFormat="1" ht="28.8">
+      <c r="A128" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B128" s="10"/>
+      <c r="C128" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D98" s="15" t="s">
+      <c r="D128" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E98" s="29"/>
-      <c r="H98" s="4" t="s">
+      <c r="E128" s="29"/>
+      <c r="H128" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:8" s="4" customFormat="1">
-      <c r="A99" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C99" s="5" t="s">
+    <row r="129" spans="1:7" s="4" customFormat="1">
+      <c r="A129" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D129" t="s">
         <v>40</v>
       </c>
-      <c r="E99"/>
-      <c r="F99"/>
-      <c r="G99"/>
-    </row>
-    <row r="100" spans="1:8" s="1" customFormat="1"/>
-    <row r="101" spans="1:8">
-      <c r="A101" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9" t="s">
+      <c r="E129"/>
+      <c r="F129"/>
+      <c r="G129"/>
+    </row>
+    <row r="130" spans="1:7" s="1" customFormat="1"/>
+    <row r="131" spans="1:7">
+      <c r="A131" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B131" s="9"/>
+      <c r="C131" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D101" s="39" t="s">
+      <c r="D131" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="E101" s="39" t="s">
+      <c r="E131" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="F101" s="12" t="s">
+      <c r="F131" s="12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
-      <c r="A102" t="s">
-        <v>2</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C102" s="5" t="s">
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C132" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D132" t="s">
         <v>153</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E132" t="s">
         <v>37</v>
       </c>
-      <c r="F102">
+      <c r="F132">
         <v>200</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new soil function for splitting soil layer
</commit_message>
<xml_diff>
--- a/Maize_Machakos/raw/Field_Overlay.xlsx
+++ b/Maize_Machakos/raw/Field_Overlay.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="199">
   <si>
     <t>cm</t>
   </si>
@@ -599,6 +599,18 @@
   </si>
   <si>
     <t>slacc</t>
+  </si>
+  <si>
+    <t>SLLB</t>
+  </si>
+  <si>
+    <t>LYRSET()</t>
+  </si>
+  <si>
+    <t>Soil Layer Depth</t>
+  </si>
+  <si>
+    <t>Soil Layer Splitting Function</t>
   </si>
 </sst>
 </file>
@@ -1077,16 +1089,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N132"/>
+  <dimension ref="A1:N135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="5.44140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="24" style="4" customWidth="1"/>
     <col min="3" max="3" width="21.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
@@ -1327,165 +1341,160 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28.8">
+    <row r="18" spans="1:9">
       <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19">
+        <v>195</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="28.8">
+      <c r="A21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="D20"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>126</v>
-      </c>
+      <c r="E21" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D22" s="37">
+      <c r="D25" s="37">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23" s="37">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="D24"/>
-    </row>
-    <row r="25" spans="1:9" ht="57.6">
-      <c r="A25" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" s="38">
-        <v>10</v>
+        <v>124</v>
+      </c>
+      <c r="D26" s="37">
+        <v>0.01</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27"/>
-      <c r="B27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:9" ht="18" customHeight="1">
+    <row r="28" spans="1:9" ht="57.6">
       <c r="A28" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="26" t="s">
-        <v>118</v>
+      <c r="B28" s="9"/>
+      <c r="C28" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>71</v>
+      </c>
+      <c r="E29" s="38">
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="B30" s="5"/>
-      <c r="C30"/>
+      <c r="A30"/>
+      <c r="B30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:9" ht="31.5" customHeight="1">
+    <row r="31" spans="1:9" ht="18" customHeight="1">
       <c r="A31" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1496,10 +1505,10 @@
         <v>12</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="2">
-        <v>500</v>
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1507,16 +1516,16 @@
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:9" ht="30.75" customHeight="1">
+    <row r="34" spans="1:9" ht="31.5" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1527,10 +1536,10 @@
         <v>12</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D35">
-        <v>0.8</v>
+        <v>113</v>
+      </c>
+      <c r="D35" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1538,110 +1547,94 @@
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:9">
-      <c r="B37" s="5"/>
-      <c r="C37"/>
-      <c r="D37"/>
-    </row>
-    <row r="38" spans="1:9" ht="16.8">
-      <c r="A38" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="21" t="s">
+    <row r="37" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A37" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="B39" s="5"/>
+      <c r="C39"/>
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="B40" s="5"/>
+      <c r="C40"/>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:9" ht="16.8">
+      <c r="A41" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="22"/>
-    </row>
-    <row r="39" spans="1:9" s="1" customFormat="1">
-      <c r="A39" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="18" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="22"/>
+    </row>
+    <row r="42" spans="1:9" s="1" customFormat="1">
+      <c r="A42" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C42" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D42" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E42" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" ht="43.2">
-      <c r="A40" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="G40" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="H40" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D41" t="s">
-        <v>165</v>
-      </c>
-      <c r="E41" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="F41" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="G41">
-        <v>25</v>
-      </c>
-      <c r="H41">
-        <v>5</v>
-      </c>
-      <c r="I41" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="B42"/>
-      <c r="D42"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-    </row>
-    <row r="43" spans="1:9" s="1" customFormat="1">
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" ht="43.2">
       <c r="A43" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="9" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>49</v>
+        <v>159</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H43" s="26" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1652,122 +1645,133 @@
         <v>12</v>
       </c>
       <c r="C44" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="G44">
+        <v>25</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="B45"/>
+      <c r="D45"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+    </row>
+    <row r="46" spans="1:9" s="1" customFormat="1">
+      <c r="A46" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D47" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="1" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A46" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9" t="s">
+    <row r="49" spans="1:13" s="1" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A49" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D49" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A47" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="5" t="s">
+    <row r="50" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D50" t="s">
         <v>131</v>
       </c>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D48">
+      <c r="D51">
         <v>990003</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="D50"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
-      <c r="L50" s="33"/>
-      <c r="M50" s="33"/>
-    </row>
-    <row r="51" spans="1:13" s="1" customFormat="1" ht="28.8">
-      <c r="A51" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51"/>
-      <c r="I51"/>
-      <c r="J51"/>
-      <c r="K51"/>
-      <c r="L51"/>
-      <c r="M51"/>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D52">
-        <v>3.5</v>
+        <v>17</v>
+      </c>
+      <c r="D52" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="D53"/>
-    </row>
-    <row r="54" spans="1:13" s="1" customFormat="1">
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+    </row>
+    <row r="54" spans="1:13" s="1" customFormat="1" ht="28.8">
       <c r="A54" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E54" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
@@ -1779,14 +1783,14 @@
       <c r="A55" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="D55">
+        <v>3.5</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -1798,11 +1802,12 @@
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57" s="2"/>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
@@ -1818,25 +1823,25 @@
         <v>12</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D58">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:13">
       <c r="D59"/>
     </row>
     <row r="60" spans="1:13" s="1" customFormat="1">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H60"/>
       <c r="I60"/>
@@ -1853,315 +1858,306 @@
         <v>12</v>
       </c>
       <c r="C61" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="D62"/>
+    </row>
+    <row r="63" spans="1:13" s="1" customFormat="1">
+      <c r="A63" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D61">
+      <c r="D64">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
-      <c r="B62"/>
-      <c r="D62"/>
-    </row>
-    <row r="64" spans="1:13" ht="16.8">
-      <c r="A64" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B64" s="21" t="s">
+    <row r="65" spans="1:14">
+      <c r="B65"/>
+      <c r="D65"/>
+    </row>
+    <row r="67" spans="1:14" ht="16.8">
+      <c r="A67" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="23"/>
-      <c r="D64" s="22"/>
-    </row>
-    <row r="65" spans="1:14">
-      <c r="A65" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="18" t="s">
+      <c r="C67" s="23"/>
+      <c r="D67" s="22"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C65" s="18" t="s">
+      <c r="C68" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D68" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="E68" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
-    </row>
-    <row r="66" spans="1:14" s="5" customFormat="1" ht="72">
-      <c r="A66" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9" t="s">
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+    </row>
+    <row r="69" spans="1:14" s="5" customFormat="1" ht="72">
+      <c r="A69" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D69" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="E69" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F66" s="16" t="s">
+      <c r="F69" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G66" s="16" t="s">
+      <c r="G69" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="H66" s="6" t="s">
+      <c r="H69" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I66" s="6" t="s">
+      <c r="I69" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="J66" s="6" t="s">
+      <c r="J69" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="K66" s="6" t="s">
+      <c r="K69" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="L66" s="6" t="s">
+      <c r="L69" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M66" s="30" t="s">
+      <c r="M69" s="30" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
-      <c r="A67" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="27" t="s">
+    <row r="70" spans="1:14">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D67" s="24" t="s">
+      <c r="D70" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E67">
-        <v>2</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="s">
         <v>79</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G70" t="s">
         <v>80</v>
       </c>
-      <c r="H67">
+      <c r="H70">
         <v>10</v>
       </c>
-      <c r="I67">
+      <c r="I70">
         <v>14</v>
       </c>
-      <c r="J67">
+      <c r="J70">
         <v>33.299999999999997</v>
       </c>
-      <c r="K67">
+      <c r="K70">
         <v>45</v>
       </c>
-      <c r="L67">
+      <c r="L70">
         <v>66.7</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
-      <c r="A68"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="24"/>
-    </row>
-    <row r="69" spans="1:14">
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-    </row>
-    <row r="70" spans="1:14" ht="16.8">
-      <c r="A70" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B70" s="21" t="s">
+    <row r="71" spans="1:14">
+      <c r="A71"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="24"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="1:14" ht="16.8">
+      <c r="A73" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C70" s="23"/>
-      <c r="D70" s="22"/>
-    </row>
-    <row r="71" spans="1:14">
-      <c r="A71" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B71" s="18" t="s">
+      <c r="C73" s="23"/>
+      <c r="D73" s="22"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C71" s="18" t="s">
+      <c r="C74" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D71" s="17" t="s">
+      <c r="D74" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="E74" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-    </row>
-    <row r="72" spans="1:14" s="5" customFormat="1" ht="57.6">
-      <c r="A72" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9" t="s">
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:14" s="5" customFormat="1" ht="57.6">
+      <c r="A75" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D75" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E75" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F75" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G72" s="6" t="s">
+      <c r="G75" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H72" s="6" t="s">
+      <c r="H75" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="I72" s="6" t="s">
+      <c r="I75" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J72" s="6" t="s">
+      <c r="J75" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="K72" s="31" t="s">
+      <c r="K75" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="L72" s="28"/>
-    </row>
-    <row r="73" spans="1:14">
-      <c r="A73" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" s="28" t="s">
+      <c r="L75" s="28"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E73">
+      <c r="E76">
         <v>-7</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F76" t="s">
         <v>35</v>
       </c>
-      <c r="G73">
+      <c r="G76">
         <v>8.3000000000000007</v>
       </c>
-      <c r="H73">
+      <c r="H76">
         <v>5</v>
       </c>
-      <c r="I73">
+      <c r="I76">
         <v>50</v>
       </c>
-      <c r="J73">
+      <c r="J76">
         <v>2.5</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="16.8">
-      <c r="A76" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B76" s="21" t="s">
+    <row r="79" spans="1:14" ht="16.8">
+      <c r="A79" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C76" s="23"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
-    </row>
-    <row r="77" spans="1:14" s="1" customFormat="1">
-      <c r="A77" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B77" s="18" t="s">
+      <c r="C79" s="23"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+    </row>
+    <row r="80" spans="1:14" s="1" customFormat="1">
+      <c r="A80" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C77" s="18" t="s">
+      <c r="C80" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D77" s="17" t="s">
+      <c r="D80" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E77" s="17" t="s">
+      <c r="E80" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F77" s="17"/>
-      <c r="G77" s="17"/>
-      <c r="M77"/>
-      <c r="N77"/>
-    </row>
-    <row r="78" spans="1:14" ht="57.6">
-      <c r="A78" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E78" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F78" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="G78" s="26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14">
-      <c r="A79" t="s">
-        <v>2</v>
-      </c>
-      <c r="B79" t="s">
-        <v>12</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79">
-        <v>20</v>
-      </c>
-      <c r="G79">
-        <v>200</v>
-      </c>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="M80"/>
+      <c r="N80"/>
     </row>
     <row r="81" spans="1:8" ht="57.6">
       <c r="A81" s="10" t="s">
@@ -2169,7 +2165,7 @@
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="9" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>55</v>
@@ -2186,132 +2182,141 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B82" t="s">
         <v>12</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>138</v>
       </c>
       <c r="E82">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F82">
         <v>20</v>
       </c>
       <c r="G82">
-        <v>100</v>
-      </c>
-      <c r="H82" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="43.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="57.6">
       <c r="A84" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E84" s="26" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="F84" s="26" t="s">
         <v>57</v>
       </c>
       <c r="G84" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="H84" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B85" t="s">
         <v>12</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E85" s="2">
-        <v>0.75</v>
+        <v>138</v>
+      </c>
+      <c r="E85">
+        <v>0.5</v>
       </c>
       <c r="F85">
         <v>20</v>
       </c>
       <c r="G85">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+        <v>100</v>
+      </c>
+      <c r="H85" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="43.2">
       <c r="A87" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E87" s="26" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F87" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="H87" s="32" t="s">
-        <v>108</v>
+        <v>57</v>
+      </c>
+      <c r="G87" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H87" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="4" t="s">
+      <c r="A88" t="s">
         <v>2</v>
       </c>
       <c r="B88" t="s">
         <v>12</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E88" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="E88" s="2">
+        <v>0.75</v>
       </c>
       <c r="F88">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="28.8">
+        <v>20</v>
+      </c>
+      <c r="G88">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B90" s="10"/>
       <c r="C90" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D90" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E90" s="36"/>
-      <c r="F90" s="36"/>
-      <c r="H90" s="32"/>
+        <v>67</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E90" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F90" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H90" s="32" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" s="4" t="s">
@@ -2321,17 +2326,17 @@
         <v>12</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D91" s="28">
-        <v>0.92</v>
-      </c>
-      <c r="F91" s="2"/>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="B92"/>
-      <c r="D92" s="28"/>
-      <c r="F92" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E91" t="s">
+        <v>66</v>
+      </c>
+      <c r="F91">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="93" spans="1:8" ht="28.8">
       <c r="A93" s="10" t="s">
@@ -2339,44 +2344,33 @@
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E93" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="F93" s="26" t="s">
-        <v>70</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D93" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E93" s="36"/>
+      <c r="F93" s="36"/>
+      <c r="H93" s="32"/>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B94" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C94" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="D94" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E94" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F94" s="42">
-        <v>0.4</v>
-      </c>
+      <c r="A94" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D94" s="28">
+        <v>0.92</v>
+      </c>
+      <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:8">
-      <c r="A95" s="24"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
+      <c r="B95"/>
+      <c r="D95" s="28"/>
       <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:8" ht="28.8">
@@ -2385,14 +2379,17 @@
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="D96" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E96" s="36"/>
-      <c r="F96" s="36"/>
-      <c r="H96" s="32"/>
+        <v>171</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E96" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="F96" s="26" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="24" t="s">
@@ -2402,13 +2399,17 @@
         <v>12</v>
       </c>
       <c r="C97" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="D97" s="28">
-        <v>40</v>
-      </c>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="D97" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E97" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F97" s="42">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="24"/>
@@ -2424,7 +2425,7 @@
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D99" s="26" t="s">
         <v>134</v>
@@ -2441,10 +2442,10 @@
         <v>12</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D100" s="28">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -2463,7 +2464,7 @@
       </c>
       <c r="B102" s="10"/>
       <c r="C102" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D102" s="26" t="s">
         <v>134</v>
@@ -2480,10 +2481,10 @@
         <v>12</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D103" s="28">
-        <v>3.5</v>
+        <v>16</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -2496,13 +2497,13 @@
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:8" ht="43.2">
+    <row r="105" spans="1:8" ht="28.8">
       <c r="A105" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D105" s="26" t="s">
         <v>134</v>
@@ -2519,10 +2520,10 @@
         <v>12</v>
       </c>
       <c r="C106" s="28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D106" s="28">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -2535,13 +2536,13 @@
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:8" ht="39" customHeight="1">
+    <row r="108" spans="1:8" ht="43.2">
       <c r="A108" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B108" s="10"/>
       <c r="C108" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D108" s="26" t="s">
         <v>134</v>
@@ -2558,7 +2559,7 @@
         <v>12</v>
       </c>
       <c r="C109" s="28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D109" s="28">
         <v>6</v>
@@ -2574,13 +2575,13 @@
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
     </row>
-    <row r="111" spans="1:8" ht="28.8">
+    <row r="111" spans="1:8" ht="39" customHeight="1">
       <c r="A111" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B111" s="10"/>
       <c r="C111" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D111" s="26" t="s">
         <v>134</v>
@@ -2597,10 +2598,10 @@
         <v>12</v>
       </c>
       <c r="C112" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="D112" s="43" t="s">
-        <v>187</v>
+        <v>184</v>
+      </c>
+      <c r="D112" s="28">
+        <v>6</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -2613,13 +2614,13 @@
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="1:8" ht="39" customHeight="1">
+    <row r="114" spans="1:8" ht="28.8">
       <c r="A114" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B114" s="10"/>
       <c r="C114" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D114" s="26" t="s">
         <v>134</v>
@@ -2636,10 +2637,10 @@
         <v>12</v>
       </c>
       <c r="C115" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="D115" s="44" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="D115" s="43" t="s">
+        <v>187</v>
       </c>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -2652,13 +2653,13 @@
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
     </row>
-    <row r="117" spans="1:8" ht="43.2">
+    <row r="117" spans="1:8" ht="39" customHeight="1">
       <c r="A117" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B117" s="10"/>
       <c r="C117" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D117" s="26" t="s">
         <v>134</v>
@@ -2675,10 +2676,10 @@
         <v>12</v>
       </c>
       <c r="C118" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="D118" s="28">
-        <v>0.06</v>
+        <v>189</v>
+      </c>
+      <c r="D118" s="44" t="s">
+        <v>190</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -2691,13 +2692,13 @@
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
     </row>
-    <row r="120" spans="1:8" ht="28.8">
+    <row r="120" spans="1:8" ht="43.2">
       <c r="A120" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B120" s="10"/>
       <c r="C120" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D120" s="26" t="s">
         <v>134</v>
@@ -2714,165 +2715,204 @@
         <v>12</v>
       </c>
       <c r="C121" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="D121" s="27">
-        <v>0.02</v>
+        <v>192</v>
+      </c>
+      <c r="D121" s="28">
+        <v>0.06</v>
       </c>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
     </row>
     <row r="122" spans="1:8">
-      <c r="B122"/>
-    </row>
-    <row r="123" spans="1:8" ht="16.8">
-      <c r="A123" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B123" s="21" t="s">
+      <c r="A122" s="24"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+    </row>
+    <row r="123" spans="1:8" ht="28.8">
+      <c r="A123" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B123" s="10"/>
+      <c r="C123" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D123" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E123" s="36"/>
+      <c r="F123" s="36"/>
+      <c r="H123" s="32"/>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C124" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="D124" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="B125"/>
+    </row>
+    <row r="126" spans="1:8" ht="16.8">
+      <c r="A126" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B126" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C123" s="22"/>
-      <c r="D123" s="22"/>
-      <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
-    </row>
-    <row r="124" spans="1:8" s="1" customFormat="1">
-      <c r="A124" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B124" s="18" t="s">
+      <c r="C126" s="22"/>
+      <c r="D126" s="22"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+    </row>
+    <row r="127" spans="1:8" s="1" customFormat="1">
+      <c r="A127" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B127" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C124" s="18" t="s">
+      <c r="C127" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D124" s="17" t="s">
+      <c r="D127" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E124" s="17" t="s">
+      <c r="E127" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F124" s="17"/>
-    </row>
-    <row r="125" spans="1:8" s="1" customFormat="1">
-      <c r="A125" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B125" s="9"/>
-      <c r="C125" s="9" t="s">
+      <c r="F127" s="17"/>
+    </row>
+    <row r="128" spans="1:8" s="1" customFormat="1">
+      <c r="A128" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B128" s="9"/>
+      <c r="C128" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D125" s="10"/>
-      <c r="E125" s="10" t="s">
+      <c r="D128" s="10"/>
+      <c r="E128" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F125" s="10" t="s">
+      <c r="F128" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H128" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
-      <c r="A126" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C126" s="5" t="s">
+    <row r="129" spans="1:8">
+      <c r="A129" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D129" t="s">
         <v>110</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E129" t="s">
         <v>37</v>
       </c>
-      <c r="F126">
+      <c r="F129">
         <v>-30</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
-      <c r="B127" s="5"/>
-      <c r="D127"/>
-    </row>
-    <row r="128" spans="1:8" s="1" customFormat="1" ht="28.8">
-      <c r="A128" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B128" s="10"/>
-      <c r="C128" s="9" t="s">
+    <row r="130" spans="1:8">
+      <c r="B130" s="5"/>
+      <c r="D130"/>
+    </row>
+    <row r="131" spans="1:8" s="1" customFormat="1" ht="28.8">
+      <c r="A131" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B131" s="10"/>
+      <c r="C131" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D128" s="15" t="s">
+      <c r="D131" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E128" s="29"/>
-      <c r="H128" s="4" t="s">
+      <c r="E131" s="29"/>
+      <c r="H131" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="129" spans="1:7" s="4" customFormat="1">
-      <c r="A129" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C129" s="5" t="s">
+    <row r="132" spans="1:8" s="4" customFormat="1">
+      <c r="A132" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C132" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D132" t="s">
         <v>40</v>
       </c>
-      <c r="E129"/>
-      <c r="F129"/>
-      <c r="G129"/>
-    </row>
-    <row r="130" spans="1:7" s="1" customFormat="1"/>
-    <row r="131" spans="1:7">
-      <c r="A131" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B131" s="9"/>
-      <c r="C131" s="9" t="s">
+      <c r="E132"/>
+      <c r="F132"/>
+      <c r="G132"/>
+    </row>
+    <row r="133" spans="1:8" s="1" customFormat="1"/>
+    <row r="134" spans="1:8">
+      <c r="A134" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B134" s="9"/>
+      <c r="C134" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D131" s="39" t="s">
+      <c r="D134" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="E131" s="39" t="s">
+      <c r="E134" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="F131" s="12" t="s">
+      <c r="F134" s="12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
-      <c r="A132" t="s">
-        <v>2</v>
-      </c>
-      <c r="B132" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C132" s="5" t="s">
+    <row r="135" spans="1:8">
+      <c r="A135" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C135" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D135" t="s">
         <v>153</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E135" t="s">
         <v>37</v>
       </c>
-      <c r="F132">
+      <c r="F135">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D54" r:id="rId1" location="Lookupcodesformanagementvariables-PLMA" display="code"/>
+    <hyperlink ref="D57" r:id="rId1" location="Lookupcodesformanagementvariables-PLMA" display="code"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Add new AUTO_IDATE function
</commit_message>
<xml_diff>
--- a/Maize_Machakos/raw/Field_Overlay.xlsx
+++ b/Maize_Machakos/raw/Field_Overlay.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="12" yWindow="-36" windowWidth="12492" windowHeight="11556"/>
   </bookViews>
   <sheets>
-    <sheet name="Field_Overlay" sheetId="6" r:id="rId1"/>
+    <sheet name="Field_Overlay" sheetId="7" r:id="rId1"/>
+    <sheet name="Field_Overlay_NoIrrigation" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="209">
   <si>
     <t>cm</t>
   </si>
@@ -611,6 +612,36 @@
   </si>
   <si>
     <t>Soil Layer Splitting Function</t>
+  </si>
+  <si>
+    <t>Irrigation Event</t>
+  </si>
+  <si>
+    <t>IDATE</t>
+  </si>
+  <si>
+    <t>Irrigation date (and other irrigation variables)</t>
+  </si>
+  <si>
+    <t>AUTO_IDATE()</t>
+  </si>
+  <si>
+    <t>Number of irrigation applications</t>
+  </si>
+  <si>
+    <t>FIELD_ORG</t>
+  </si>
+  <si>
+    <t>Base Temperature(oC)</t>
+  </si>
+  <si>
+    <t>IRVAL - Irrigation amount, depth of water (mm)</t>
+  </si>
+  <si>
+    <t>#1 irrigation -Cumulative value of Growing degree-day</t>
+  </si>
+  <si>
+    <t>! The value is not reasonable, just show the idea of function</t>
   </si>
 </sst>
 </file>
@@ -1088,11 +1119,1951 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N141"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="5.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="12" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.8">
+      <c r="A1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="34" t="str">
+        <f>CONCATENATE(D3,"-",D4,"-",D5,"-",D6,"-",D7,"-",D8)</f>
+        <v>MACHAKOS-1----FIELD</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="5"/>
+      <c r="C9"/>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="16.8">
+      <c r="A10" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15"/>
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:6" ht="16.8">
+      <c r="A16" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1">
+      <c r="A17" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="28.8">
+      <c r="A21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="37">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:9" ht="57.6">
+      <c r="A28" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" customHeight="1">
+      <c r="A31" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="B33" s="5"/>
+      <c r="C33"/>
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="1:9" ht="31.5" customHeight="1">
+      <c r="A34" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="B36" s="5"/>
+      <c r="C36"/>
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A37" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="B39" s="5"/>
+      <c r="C39"/>
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="B40" s="5"/>
+      <c r="C40"/>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:9" ht="16.8">
+      <c r="A41" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="22"/>
+    </row>
+    <row r="42" spans="1:9" s="1" customFormat="1">
+      <c r="A42" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" ht="43.2">
+      <c r="A43" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H43" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="G44">
+        <v>25</v>
+      </c>
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="B45"/>
+      <c r="D45"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+    </row>
+    <row r="46" spans="1:9" s="1" customFormat="1">
+      <c r="A46" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="1" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A49" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>990003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="D53"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+    </row>
+    <row r="54" spans="1:13" s="1" customFormat="1" ht="28.8">
+      <c r="A54" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="1:13" s="1" customFormat="1">
+      <c r="A57" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="1:13" s="1" customFormat="1">
+      <c r="A60" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="D62"/>
+    </row>
+    <row r="63" spans="1:13" s="1" customFormat="1">
+      <c r="A63" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63"/>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D64">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="B65"/>
+      <c r="D65"/>
+    </row>
+    <row r="67" spans="1:13" ht="16.8">
+      <c r="A67" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="23"/>
+      <c r="D67" s="22"/>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+    </row>
+    <row r="69" spans="1:13" s="5" customFormat="1" ht="72">
+      <c r="A69" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="L69" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="M69" s="30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D70" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="s">
+        <v>79</v>
+      </c>
+      <c r="G70" t="s">
+        <v>80</v>
+      </c>
+      <c r="H70">
+        <v>10</v>
+      </c>
+      <c r="I70">
+        <v>14</v>
+      </c>
+      <c r="J70">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="K70">
+        <v>45</v>
+      </c>
+      <c r="L70">
+        <v>66.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="24"/>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="1:13" ht="16.8">
+      <c r="A73" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" s="23"/>
+      <c r="D73" s="22"/>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="1:13" s="5" customFormat="1" ht="57.6">
+      <c r="A75" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J75" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K75" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="L75" s="28"/>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E76">
+        <v>-7</v>
+      </c>
+      <c r="F76" t="s">
+        <v>35</v>
+      </c>
+      <c r="G76">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H76">
+        <v>5</v>
+      </c>
+      <c r="I76">
+        <v>50</v>
+      </c>
+      <c r="J76">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="16.8">
+      <c r="A79" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C79" s="23"/>
+      <c r="D79" s="22"/>
+    </row>
+    <row r="80" spans="1:13">
+      <c r="A80" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D80" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="1:14" s="5" customFormat="1" ht="72">
+      <c r="A81" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="F81" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="G81" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I81" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K81" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="L81"/>
+    </row>
+    <row r="82" spans="1:14">
+      <c r="A82" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E82">
+        <v>2</v>
+      </c>
+      <c r="F82">
+        <v>5</v>
+      </c>
+      <c r="G82">
+        <v>400</v>
+      </c>
+      <c r="H82">
+        <v>50</v>
+      </c>
+      <c r="I82">
+        <v>160</v>
+      </c>
+      <c r="J82">
+        <v>40</v>
+      </c>
+      <c r="K82" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="A83"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="24"/>
+    </row>
+    <row r="84" spans="1:14">
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+    </row>
+    <row r="85" spans="1:14" ht="16.8">
+      <c r="A85" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="23"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="M85" s="1"/>
+      <c r="N85" s="1"/>
+    </row>
+    <row r="86" spans="1:14" s="1" customFormat="1">
+      <c r="A86" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" s="17"/>
+      <c r="G86" s="17"/>
+      <c r="M86"/>
+      <c r="N86"/>
+    </row>
+    <row r="87" spans="1:14" ht="57.6">
+      <c r="A87" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="10"/>
+      <c r="C87" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F87" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G87" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14">
+      <c r="A88" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>20</v>
+      </c>
+      <c r="G88">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" ht="57.6">
+      <c r="A90" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="10"/>
+      <c r="C90" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E90" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F90" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G90" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14">
+      <c r="A91" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E91">
+        <v>0.5</v>
+      </c>
+      <c r="F91">
+        <v>20</v>
+      </c>
+      <c r="G91">
+        <v>100</v>
+      </c>
+      <c r="H91" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="43.2">
+      <c r="A93" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="10"/>
+      <c r="C93" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E93" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F93" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G93" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H93" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14">
+      <c r="A94" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" t="s">
+        <v>12</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E94" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F94">
+        <v>20</v>
+      </c>
+      <c r="G94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14">
+      <c r="A96" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E96" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F96" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H96" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" t="s">
+        <v>12</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E97" t="s">
+        <v>66</v>
+      </c>
+      <c r="F97">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="28.8">
+      <c r="A99" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" s="10"/>
+      <c r="C99" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D99" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E99" s="36"/>
+      <c r="F99" s="36"/>
+      <c r="H99" s="32"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D100" s="28">
+        <v>0.92</v>
+      </c>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="B101"/>
+      <c r="D101" s="28"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:8" ht="28.8">
+      <c r="A102" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B102" s="10"/>
+      <c r="C102" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E102" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="F102" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D103" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E103" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F103" s="42">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="24"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+    </row>
+    <row r="105" spans="1:8" ht="28.8">
+      <c r="A105" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="10"/>
+      <c r="C105" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D105" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E105" s="36"/>
+      <c r="F105" s="36"/>
+      <c r="H105" s="32"/>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D106" s="28">
+        <v>40</v>
+      </c>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="24"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+    </row>
+    <row r="108" spans="1:8" ht="28.8">
+      <c r="A108" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" s="10"/>
+      <c r="C108" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D108" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E108" s="36"/>
+      <c r="F108" s="36"/>
+      <c r="H108" s="32"/>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="D109" s="28">
+        <v>16</v>
+      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="24"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+    </row>
+    <row r="111" spans="1:8" ht="28.8">
+      <c r="A111" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" s="10"/>
+      <c r="C111" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D111" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E111" s="36"/>
+      <c r="F111" s="36"/>
+      <c r="H111" s="32"/>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C112" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D112" s="28">
+        <v>3.5</v>
+      </c>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="24"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+    </row>
+    <row r="114" spans="1:8" ht="43.2">
+      <c r="A114" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="10"/>
+      <c r="C114" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D114" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E114" s="36"/>
+      <c r="F114" s="36"/>
+      <c r="H114" s="32"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="D115" s="28">
+        <v>6</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="24"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+    </row>
+    <row r="117" spans="1:8" ht="39" customHeight="1">
+      <c r="A117" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B117" s="10"/>
+      <c r="C117" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D117" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E117" s="36"/>
+      <c r="F117" s="36"/>
+      <c r="H117" s="32"/>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D118" s="28">
+        <v>6</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" s="24"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+    </row>
+    <row r="120" spans="1:8" ht="28.8">
+      <c r="A120" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="10"/>
+      <c r="C120" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D120" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E120" s="36"/>
+      <c r="F120" s="36"/>
+      <c r="H120" s="32"/>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D121" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" s="24"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+    </row>
+    <row r="123" spans="1:8" ht="39" customHeight="1">
+      <c r="A123" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B123" s="10"/>
+      <c r="C123" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D123" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E123" s="36"/>
+      <c r="F123" s="36"/>
+      <c r="H123" s="32"/>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C124" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="D124" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" s="24"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="28"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+    </row>
+    <row r="126" spans="1:8" ht="43.2">
+      <c r="A126" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B126" s="10"/>
+      <c r="C126" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D126" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E126" s="36"/>
+      <c r="F126" s="36"/>
+      <c r="H126" s="32"/>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B127" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C127" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D127" s="28">
+        <v>0.06</v>
+      </c>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" s="24"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+    </row>
+    <row r="129" spans="1:8" ht="28.8">
+      <c r="A129" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B129" s="10"/>
+      <c r="C129" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D129" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E129" s="36"/>
+      <c r="F129" s="36"/>
+      <c r="H129" s="32"/>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="D130" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="B131"/>
+    </row>
+    <row r="132" spans="1:8" ht="16.8">
+      <c r="A132" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B132" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C132" s="22"/>
+      <c r="D132" s="22"/>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+    </row>
+    <row r="133" spans="1:8" s="1" customFormat="1">
+      <c r="A133" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B133" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C133" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D133" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E133" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F133" s="17"/>
+    </row>
+    <row r="134" spans="1:8" s="1" customFormat="1">
+      <c r="A134" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B134" s="9"/>
+      <c r="C134" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D134" s="10"/>
+      <c r="E134" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F134" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H134" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D135" t="s">
+        <v>110</v>
+      </c>
+      <c r="E135" t="s">
+        <v>37</v>
+      </c>
+      <c r="F135">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="B136" s="5"/>
+      <c r="D136"/>
+    </row>
+    <row r="137" spans="1:8" s="1" customFormat="1" ht="28.8">
+      <c r="A137" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B137" s="10"/>
+      <c r="C137" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E137" s="29"/>
+      <c r="H137" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" s="4" customFormat="1">
+      <c r="A138" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D138" t="s">
+        <v>40</v>
+      </c>
+      <c r="E138"/>
+      <c r="F138"/>
+      <c r="G138"/>
+    </row>
+    <row r="139" spans="1:8" s="1" customFormat="1"/>
+    <row r="140" spans="1:8">
+      <c r="A140" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140" s="9"/>
+      <c r="C140" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D140" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="E140" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="F140" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D141" t="s">
+        <v>153</v>
+      </c>
+      <c r="E141" t="s">
+        <v>37</v>
+      </c>
+      <c r="F141">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D57" r:id="rId1" location="Lookupcodesformanagementvariables-PLMA" display="code"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1134,7 +3105,7 @@
       </c>
       <c r="D2" s="34" t="str">
         <f>CONCATENATE(D3,"-",D4,"-",D5,"-",D6,"-",D7,"-",D8)</f>
-        <v>MACHAKOS-1----FIELD</v>
+        <v>MACHAKOS-1----FIELD_ORG</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>123</v>
@@ -1231,7 +3202,7 @@
         <v>127</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>204</v>
       </c>
       <c r="E8" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
Add example for TRANSPOSE()
</commit_message>
<xml_diff>
--- a/Maize_Machakos/raw/Field_Overlay.xlsx
+++ b/Maize_Machakos/raw/Field_Overlay.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="232">
   <si>
     <t>cm</t>
   </si>
@@ -642,6 +642,75 @@
   </si>
   <si>
     <t>! The value is not reasonable, just show the idea of function</t>
+  </si>
+  <si>
+    <t>SLFIC</t>
+  </si>
+  <si>
+    <t>Inert organic C Fraction array (%)</t>
+  </si>
+  <si>
+    <t>! Inert C</t>
+  </si>
+  <si>
+    <t>$SLFIC</t>
+  </si>
+  <si>
+    <t>OFFSET()</t>
+  </si>
+  <si>
+    <t>offset value</t>
+  </si>
+  <si>
+    <t>Offset function</t>
+  </si>
+  <si>
+    <t>SLFAC</t>
+  </si>
+  <si>
+    <t>! Biom</t>
+  </si>
+  <si>
+    <t>! KL</t>
+  </si>
+  <si>
+    <t>Biologically active soil organic carbon by layer, fraction of total (%)</t>
+  </si>
+  <si>
+    <t>SLSAT</t>
+  </si>
+  <si>
+    <t>$SLBDM</t>
+  </si>
+  <si>
+    <t>! Saturtion</t>
+  </si>
+  <si>
+    <t>$SLSAT</t>
+  </si>
+  <si>
+    <t>SLDRL</t>
+  </si>
+  <si>
+    <t>Drainage rate as fraction per day, per layer (1/d)</t>
+  </si>
+  <si>
+    <t>Insert array value function</t>
+  </si>
+  <si>
+    <t>TRANSPOSE()</t>
+  </si>
+  <si>
+    <t>Value for layer 1</t>
+  </si>
+  <si>
+    <t>Value for layer 2</t>
+  </si>
+  <si>
+    <t>Value for layer 3</t>
+  </si>
+  <si>
+    <t>Value for layer 4</t>
   </si>
 </sst>
 </file>
@@ -1119,9 +1188,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N141"/>
+  <dimension ref="A1:N163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -1131,11 +1202,12 @@
     <col min="4" max="4" width="25.109375" style="5" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
     <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="12" width="15" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.8">
@@ -1369,191 +1441,213 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="43.2">
       <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="9" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>198</v>
+        <v>226</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="28.8">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19">
+        <v>0.4</v>
+      </c>
+      <c r="F19">
+        <v>0.3</v>
+      </c>
+      <c r="G19">
+        <v>0.2</v>
+      </c>
+      <c r="H19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="B20"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22">
+        <v>195</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="28.8">
+      <c r="A24" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="D23"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>126</v>
-      </c>
+      <c r="E24" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="37">
+      <c r="D28" s="37">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="37">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="1:9" ht="57.6">
-      <c r="A28" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="38">
-        <v>10</v>
+        <v>124</v>
+      </c>
+      <c r="D29" s="37">
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30"/>
-      <c r="B30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:9" ht="18" customHeight="1">
+    <row r="31" spans="1:9" ht="57.6">
       <c r="A31" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>118</v>
+      <c r="B31" s="9"/>
+      <c r="C31" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>117</v>
+        <v>71</v>
+      </c>
+      <c r="E32" s="38">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="B33" s="5"/>
-      <c r="C33"/>
+      <c r="A33"/>
+      <c r="B33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:9" ht="31.5" customHeight="1">
+    <row r="34" spans="1:9" ht="18" customHeight="1">
       <c r="A34" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1564,10 +1658,10 @@
         <v>12</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D35" s="2">
-        <v>500</v>
+        <v>116</v>
+      </c>
+      <c r="D35" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1575,16 +1669,16 @@
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:9" ht="30.75" customHeight="1">
+    <row r="37" spans="1:9" ht="31.5" customHeight="1">
       <c r="A37" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1595,10 +1689,10 @@
         <v>12</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D38">
-        <v>0.8</v>
+        <v>113</v>
+      </c>
+      <c r="D38" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1606,110 +1700,94 @@
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:9">
-      <c r="B40" s="5"/>
-      <c r="C40"/>
-      <c r="D40"/>
-    </row>
-    <row r="41" spans="1:9" ht="16.8">
-      <c r="A41" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="21" t="s">
+    <row r="40" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A40" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="B42" s="5"/>
+      <c r="C42"/>
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="B43" s="5"/>
+      <c r="C43"/>
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="1:9" ht="16.8">
+      <c r="A44" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="22"/>
-    </row>
-    <row r="42" spans="1:9" s="1" customFormat="1">
-      <c r="A42" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="18" t="s">
+      <c r="C44" s="23"/>
+      <c r="D44" s="22"/>
+    </row>
+    <row r="45" spans="1:9" s="1" customFormat="1">
+      <c r="A45" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C45" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D45" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E45" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" ht="43.2">
-      <c r="A43" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="G43" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="H43" s="26" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D44" t="s">
-        <v>165</v>
-      </c>
-      <c r="E44" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="F44" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="G44">
-        <v>25</v>
-      </c>
-      <c r="H44">
-        <v>5</v>
-      </c>
-      <c r="I44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="B45"/>
-      <c r="D45"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-    </row>
-    <row r="46" spans="1:9" s="1" customFormat="1">
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" ht="43.2">
       <c r="A46" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="9" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>49</v>
+        <v>159</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G46" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H46" s="26" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1720,122 +1798,133 @@
         <v>12</v>
       </c>
       <c r="C47" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="F47" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="G47">
+        <v>25</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="B48"/>
+      <c r="D48"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+    </row>
+    <row r="49" spans="1:13" s="1" customFormat="1">
+      <c r="A49" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D50" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="1" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A49" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9" t="s">
+    <row r="52" spans="1:13" s="1" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A52" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D52" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A50" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="5" t="s">
+    <row r="53" spans="1:13" s="1" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D53" t="s">
         <v>131</v>
       </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="5" t="s">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D51">
+      <c r="D54">
         <v>990003</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="D53"/>
-      <c r="I53" s="33"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="33"/>
-      <c r="L53" s="33"/>
-      <c r="M53" s="33"/>
-    </row>
-    <row r="54" spans="1:13" s="1" customFormat="1" ht="28.8">
-      <c r="A54" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H54"/>
-      <c r="I54"/>
-      <c r="J54"/>
-      <c r="K54"/>
-      <c r="L54"/>
-      <c r="M54"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D55">
-        <v>3.5</v>
+        <v>17</v>
+      </c>
+      <c r="D55" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="D56"/>
-    </row>
-    <row r="57" spans="1:13" s="1" customFormat="1">
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+    </row>
+    <row r="57" spans="1:13" s="1" customFormat="1" ht="28.8">
       <c r="A57" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E57" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
@@ -1847,14 +1936,14 @@
       <c r="A58" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="D58">
+        <v>3.5</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -1866,11 +1955,12 @@
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E60" s="2"/>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60"/>
@@ -1886,25 +1976,25 @@
         <v>12</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D61">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="D61" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:13">
       <c r="D62"/>
     </row>
     <row r="63" spans="1:13" s="1" customFormat="1">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H63"/>
       <c r="I63"/>
@@ -1921,425 +2011,416 @@
         <v>12</v>
       </c>
       <c r="C64" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="1:13" s="1" customFormat="1">
+      <c r="A66" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D64">
+      <c r="D67">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
-      <c r="B65"/>
-      <c r="D65"/>
-    </row>
-    <row r="67" spans="1:13" ht="16.8">
-      <c r="A67" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" s="21" t="s">
+    <row r="68" spans="1:13">
+      <c r="B68"/>
+      <c r="D68"/>
+    </row>
+    <row r="70" spans="1:13" ht="16.8">
+      <c r="A70" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="22"/>
-    </row>
-    <row r="68" spans="1:13">
-      <c r="A68" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="18" t="s">
+      <c r="C70" s="23"/>
+      <c r="D70" s="22"/>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C68" s="18" t="s">
+      <c r="C71" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="D71" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E68" s="17" t="s">
+      <c r="E71" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
-    </row>
-    <row r="69" spans="1:13" s="5" customFormat="1" ht="72">
-      <c r="A69" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9" t="s">
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+    </row>
+    <row r="72" spans="1:13" s="5" customFormat="1" ht="72">
+      <c r="A72" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D72" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E69" s="6" t="s">
+      <c r="E72" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="F69" s="16" t="s">
+      <c r="F72" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G69" s="16" t="s">
+      <c r="G72" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="H69" s="6" t="s">
+      <c r="H72" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I69" s="6" t="s">
+      <c r="I72" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="J69" s="6" t="s">
+      <c r="J72" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="K69" s="6" t="s">
+      <c r="K72" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="L69" s="6" t="s">
+      <c r="L72" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M69" s="30" t="s">
+      <c r="M72" s="30" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
-      <c r="A70" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C70" s="27" t="s">
+    <row r="73" spans="1:13">
+      <c r="A73" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D70" s="24" t="s">
+      <c r="D73" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E70">
-        <v>2</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73" t="s">
         <v>79</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G73" t="s">
         <v>80</v>
       </c>
-      <c r="H70">
+      <c r="H73">
         <v>10</v>
       </c>
-      <c r="I70">
+      <c r="I73">
         <v>14</v>
       </c>
-      <c r="J70">
+      <c r="J73">
         <v>33.299999999999997</v>
       </c>
-      <c r="K70">
+      <c r="K73">
         <v>45</v>
       </c>
-      <c r="L70">
+      <c r="L73">
         <v>66.7</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
-      <c r="A71"/>
-      <c r="C71" s="27"/>
-      <c r="D71" s="24"/>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-    </row>
-    <row r="73" spans="1:13" ht="16.8">
-      <c r="A73" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="21" t="s">
+    <row r="74" spans="1:13">
+      <c r="A74"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="24"/>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:13" ht="16.8">
+      <c r="A76" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="22"/>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" s="18" t="s">
+      <c r="C76" s="23"/>
+      <c r="D76" s="22"/>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="18" t="s">
+      <c r="C77" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D74" s="17" t="s">
+      <c r="D77" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="E77" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="2"/>
-      <c r="L74" s="2"/>
-    </row>
-    <row r="75" spans="1:13" s="5" customFormat="1" ht="57.6">
-      <c r="A75" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9" t="s">
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="1:13" s="5" customFormat="1" ht="57.6">
+      <c r="A78" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D78" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E75" s="6" t="s">
+      <c r="E78" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F75" s="16" t="s">
+      <c r="F78" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G75" s="6" t="s">
+      <c r="G78" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H75" s="6" t="s">
+      <c r="H78" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="I75" s="6" t="s">
+      <c r="I78" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="J75" s="6" t="s">
+      <c r="J78" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="K75" s="31" t="s">
+      <c r="K78" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="L75" s="28"/>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="A76" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C76" s="28" t="s">
+      <c r="L78" s="28"/>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E76">
+      <c r="E79">
         <v>-7</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F79" t="s">
         <v>35</v>
       </c>
-      <c r="G76">
+      <c r="G79">
         <v>8.3000000000000007</v>
       </c>
-      <c r="H76">
+      <c r="H79">
         <v>5</v>
       </c>
-      <c r="I76">
+      <c r="I79">
         <v>50</v>
       </c>
-      <c r="J76">
+      <c r="J79">
         <v>2.5</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="16.8">
-      <c r="A79" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B79" s="21" t="s">
+    <row r="82" spans="1:14" ht="16.8">
+      <c r="A82" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="C79" s="23"/>
-      <c r="D79" s="22"/>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="A80" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B80" s="18" t="s">
+      <c r="C82" s="23"/>
+      <c r="D82" s="22"/>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="A83" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C80" s="18" t="s">
+      <c r="C83" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D80" s="17" t="s">
+      <c r="D83" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E80" s="17" t="s">
+      <c r="E83" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-    </row>
-    <row r="81" spans="1:14" s="5" customFormat="1" ht="72">
-      <c r="A81" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9" t="s">
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="1:14" s="5" customFormat="1" ht="57.6">
+      <c r="A84" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D81" s="9" t="s">
+      <c r="D84" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E84" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="F81" s="16" t="s">
+      <c r="F84" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="G81" s="16" t="s">
+      <c r="G84" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="H81" s="6" t="s">
+      <c r="H84" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="I81" s="16" t="s">
+      <c r="I84" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="J81" s="6" t="s">
+      <c r="J84" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="K81" s="30" t="s">
+      <c r="K84" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="L81"/>
-    </row>
-    <row r="82" spans="1:14">
-      <c r="A82" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82" s="28" t="s">
+      <c r="L84"/>
+    </row>
+    <row r="85" spans="1:14">
+      <c r="A85" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E82">
-        <v>2</v>
-      </c>
-      <c r="F82">
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85">
         <v>5</v>
       </c>
-      <c r="G82">
+      <c r="G85">
         <v>400</v>
       </c>
-      <c r="H82">
+      <c r="H85">
         <v>50</v>
       </c>
-      <c r="I82">
+      <c r="I85">
         <v>160</v>
       </c>
-      <c r="J82">
+      <c r="J85">
         <v>40</v>
       </c>
-      <c r="K82" t="s">
+      <c r="K85" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
-      <c r="A83"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="24"/>
-    </row>
-    <row r="84" spans="1:14">
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
-    </row>
-    <row r="85" spans="1:14" ht="16.8">
-      <c r="A85" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B85" s="21" t="s">
+    <row r="86" spans="1:14">
+      <c r="A86"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="24"/>
+    </row>
+    <row r="87" spans="1:14">
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="1:14" ht="16.8">
+      <c r="A88" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="23"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="M85" s="1"/>
-      <c r="N85" s="1"/>
-    </row>
-    <row r="86" spans="1:14" s="1" customFormat="1">
-      <c r="A86" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B86" s="18" t="s">
+      <c r="C88" s="23"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+    </row>
+    <row r="89" spans="1:14" s="1" customFormat="1">
+      <c r="A89" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="C89" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D86" s="17" t="s">
+      <c r="D89" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E86" s="17" t="s">
+      <c r="E89" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F86" s="17"/>
-      <c r="G86" s="17"/>
-      <c r="M86"/>
-      <c r="N86"/>
-    </row>
-    <row r="87" spans="1:14" ht="57.6">
-      <c r="A87" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B87" s="10"/>
-      <c r="C87" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E87" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F87" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="G87" s="26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14">
-      <c r="A88" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E88">
-        <v>1</v>
-      </c>
-      <c r="F88">
-        <v>20</v>
-      </c>
-      <c r="G88">
-        <v>200</v>
-      </c>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="M89"/>
+      <c r="N89"/>
     </row>
     <row r="90" spans="1:14" ht="57.6">
       <c r="A90" s="10" t="s">
@@ -2347,7 +2428,7 @@
       </c>
       <c r="B90" s="10"/>
       <c r="C90" s="9" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>55</v>
@@ -2364,152 +2445,161 @@
     </row>
     <row r="91" spans="1:14">
       <c r="A91" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
         <v>12</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>138</v>
       </c>
       <c r="E91">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F91">
         <v>20</v>
       </c>
       <c r="G91">
-        <v>100</v>
-      </c>
-      <c r="H91" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" ht="43.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" ht="57.6">
       <c r="A93" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E93" s="26" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="E93" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="F93" s="26" t="s">
         <v>57</v>
       </c>
       <c r="G93" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="H93" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
     </row>
     <row r="94" spans="1:14">
       <c r="A94" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B94" t="s">
         <v>12</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E94" s="2">
-        <v>0.75</v>
+        <v>138</v>
+      </c>
+      <c r="E94">
+        <v>0.5</v>
       </c>
       <c r="F94">
         <v>20</v>
       </c>
       <c r="G94">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14">
+        <v>100</v>
+      </c>
+      <c r="H94" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" ht="43.2">
       <c r="A96" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E96" s="26" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F96" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="H96" s="32" t="s">
-        <v>108</v>
+        <v>57</v>
+      </c>
+      <c r="G96" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H96" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:8">
-      <c r="A97" s="4" t="s">
+      <c r="A97" t="s">
         <v>2</v>
       </c>
       <c r="B97" t="s">
         <v>12</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E97" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="E97" s="2">
+        <v>0.75</v>
       </c>
       <c r="F97">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="28.8">
+        <v>20</v>
+      </c>
+      <c r="G97">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B99" s="10"/>
       <c r="C99" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D99" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E99" s="36"/>
-      <c r="F99" s="36"/>
-      <c r="H99" s="32"/>
+        <v>67</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E99" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F99" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H99" s="32" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="100" spans="1:8">
-      <c r="A100" s="4" t="s">
-        <v>2</v>
+      <c r="A100" t="s">
+        <v>1</v>
       </c>
       <c r="B100" t="s">
         <v>12</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D100" s="28">
-        <v>0.92</v>
-      </c>
-      <c r="F100" s="2"/>
-    </row>
-    <row r="101" spans="1:8">
-      <c r="B101"/>
-      <c r="D101" s="28"/>
-      <c r="F101" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E100" t="s">
+        <v>66</v>
+      </c>
+      <c r="F100">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="102" spans="1:8" ht="28.8">
       <c r="A102" s="10" t="s">
@@ -2517,123 +2607,169 @@
       </c>
       <c r="B102" s="10"/>
       <c r="C102" s="9" t="s">
-        <v>171</v>
+        <v>210</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E102" s="26" t="s">
-        <v>172</v>
+      <c r="E102" s="9" t="s">
+        <v>210</v>
       </c>
       <c r="F102" s="26" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:8">
-      <c r="A103" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C103" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="D103" s="27" t="s">
+      <c r="A103" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" t="s">
+        <v>31</v>
+      </c>
+      <c r="C103" t="s">
+        <v>220</v>
+      </c>
+      <c r="D103" t="s">
         <v>65</v>
       </c>
-      <c r="E103" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="F103" s="42">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
-      <c r="A104" s="24"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-    </row>
-    <row r="105" spans="1:8" ht="28.8">
-      <c r="A105" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B105" s="10"/>
-      <c r="C105" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="D105" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E105" s="36"/>
-      <c r="F105" s="36"/>
-      <c r="H105" s="32"/>
-    </row>
-    <row r="106" spans="1:8">
-      <c r="A106" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C106" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="D106" s="28">
-        <v>40</v>
-      </c>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
+      <c r="E103" t="s">
+        <v>221</v>
+      </c>
+      <c r="F103">
+        <v>-0.377</v>
+      </c>
+      <c r="H103" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="28.8">
+      <c r="A104" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B104" s="10"/>
+      <c r="C104" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F104" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" t="s">
+        <v>31</v>
+      </c>
+      <c r="C105" t="s">
+        <v>220</v>
+      </c>
+      <c r="D105" t="s">
+        <v>213</v>
+      </c>
+      <c r="E105" t="s">
+        <v>223</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="H105" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="28.8">
+      <c r="A106" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B106" s="10"/>
+      <c r="C106" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F106" s="26" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="107" spans="1:8">
-      <c r="A107" s="24"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-    </row>
-    <row r="108" spans="1:8" ht="28.8">
-      <c r="A108" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B108" s="10"/>
-      <c r="C108" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D108" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E108" s="36"/>
-      <c r="F108" s="36"/>
-      <c r="H108" s="32"/>
-    </row>
-    <row r="109" spans="1:8">
-      <c r="A109" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C109" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="D109" s="28">
-        <v>16</v>
-      </c>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
+      <c r="A107" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" t="s">
+        <v>31</v>
+      </c>
+      <c r="C107" t="s">
+        <v>220</v>
+      </c>
+      <c r="D107" t="s">
+        <v>65</v>
+      </c>
+      <c r="E107" t="s">
+        <v>223</v>
+      </c>
+      <c r="F107">
+        <v>0.95</v>
+      </c>
+      <c r="H107" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="57.6">
+      <c r="A109" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" s="10"/>
+      <c r="C109" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E109" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F109" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G109" s="26" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="110" spans="1:8">
-      <c r="A110" s="24"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="2"/>
-      <c r="F110" s="2"/>
+      <c r="A110" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" t="s">
+        <v>209</v>
+      </c>
+      <c r="D110" t="s">
+        <v>138</v>
+      </c>
+      <c r="E110">
+        <v>0.6</v>
+      </c>
+      <c r="F110">
+        <v>15</v>
+      </c>
+      <c r="G110">
+        <v>150</v>
+      </c>
+      <c r="H110" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="111" spans="1:8" ht="28.8">
       <c r="A111" s="10" t="s">
@@ -2641,416 +2777,759 @@
       </c>
       <c r="B111" s="10"/>
       <c r="C111" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D111" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F111" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" t="s">
+        <v>31</v>
+      </c>
+      <c r="C112" t="s">
+        <v>209</v>
+      </c>
+      <c r="D112" t="s">
+        <v>65</v>
+      </c>
+      <c r="E112" t="s">
+        <v>212</v>
+      </c>
+      <c r="F112">
+        <v>-1</v>
+      </c>
+      <c r="H112" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="28.8">
+      <c r="A113" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B113" s="10"/>
+      <c r="C113" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F113" s="26" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" t="s">
+        <v>209</v>
+      </c>
+      <c r="D114" t="s">
+        <v>213</v>
+      </c>
+      <c r="E114" t="s">
+        <v>212</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="H114" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="28.8">
+      <c r="A116" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B116" s="10"/>
+      <c r="C116" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D116" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="E111" s="36"/>
-      <c r="F111" s="36"/>
-      <c r="H111" s="32"/>
-    </row>
-    <row r="112" spans="1:8">
-      <c r="A112" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C112" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="D112" s="28">
-        <v>3.5</v>
-      </c>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-    </row>
-    <row r="113" spans="1:8">
-      <c r="A113" s="24"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-    </row>
-    <row r="114" spans="1:8" ht="43.2">
-      <c r="A114" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B114" s="10"/>
-      <c r="C114" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D114" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E114" s="36"/>
-      <c r="F114" s="36"/>
-      <c r="H114" s="32"/>
-    </row>
-    <row r="115" spans="1:8">
-      <c r="A115" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C115" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="D115" s="28">
-        <v>6</v>
-      </c>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-    </row>
-    <row r="116" spans="1:8">
-      <c r="A116" s="24"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-    </row>
-    <row r="117" spans="1:8" ht="39" customHeight="1">
-      <c r="A117" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B117" s="10"/>
-      <c r="C117" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D117" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E117" s="36"/>
-      <c r="F117" s="36"/>
-      <c r="H117" s="32"/>
+      <c r="E116" s="36"/>
+      <c r="F116" s="36"/>
+      <c r="H116" s="32"/>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" t="s">
+        <v>12</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D117" s="28">
+        <v>0.92</v>
+      </c>
+      <c r="F117" s="2"/>
     </row>
     <row r="118" spans="1:8">
-      <c r="A118" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B118" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C118" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="D118" s="28">
-        <v>6</v>
-      </c>
-      <c r="E118" s="2"/>
+      <c r="B118"/>
+      <c r="D118" s="28"/>
       <c r="F118" s="2"/>
     </row>
-    <row r="119" spans="1:8">
-      <c r="A119" s="24"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="28"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-    </row>
-    <row r="120" spans="1:8" ht="28.8">
-      <c r="A120" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B120" s="10"/>
-      <c r="C120" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D120" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="E120" s="36"/>
-      <c r="F120" s="36"/>
-      <c r="H120" s="32"/>
+    <row r="119" spans="1:8" ht="28.8">
+      <c r="A119" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="10"/>
+      <c r="C119" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D119" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E119" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="F119" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C120" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D120" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E120" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F120" s="42">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="121" spans="1:8">
-      <c r="A121" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B121" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C121" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="D121" s="43" t="s">
-        <v>187</v>
-      </c>
+      <c r="A121" s="24"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
     </row>
-    <row r="122" spans="1:8">
-      <c r="A122" s="24"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="28"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-    </row>
-    <row r="123" spans="1:8" ht="39" customHeight="1">
-      <c r="A123" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B123" s="10"/>
-      <c r="C123" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="D123" s="26" t="s">
+    <row r="122" spans="1:8" ht="28.8">
+      <c r="A122" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B122" s="10"/>
+      <c r="C122" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D122" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="E123" s="36"/>
-      <c r="F123" s="36"/>
-      <c r="H123" s="32"/>
+      <c r="E122" s="36"/>
+      <c r="F122" s="36"/>
+      <c r="H122" s="32"/>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C123" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="D123" s="28">
+        <v>40</v>
+      </c>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:8">
-      <c r="A124" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B124" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C124" s="28" t="s">
-        <v>189</v>
-      </c>
-      <c r="D124" s="44" t="s">
-        <v>190</v>
-      </c>
+      <c r="A124" s="24"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
     </row>
-    <row r="125" spans="1:8">
-      <c r="A125" s="24"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="28"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
-    </row>
-    <row r="126" spans="1:8" ht="43.2">
-      <c r="A126" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B126" s="10"/>
-      <c r="C126" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="D126" s="26" t="s">
+    <row r="125" spans="1:8" ht="28.8">
+      <c r="A125" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B125" s="10"/>
+      <c r="C125" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D125" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="E126" s="36"/>
-      <c r="F126" s="36"/>
-      <c r="H126" s="32"/>
+      <c r="E125" s="36"/>
+      <c r="F125" s="36"/>
+      <c r="H125" s="32"/>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="D126" s="28">
+        <v>16</v>
+      </c>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
     </row>
     <row r="127" spans="1:8">
-      <c r="A127" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B127" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C127" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="D127" s="28">
-        <v>0.06</v>
-      </c>
+      <c r="A127" s="24"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="28"/>
+      <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
     </row>
-    <row r="128" spans="1:8">
-      <c r="A128" s="24"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="28"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-    </row>
-    <row r="129" spans="1:8" ht="28.8">
-      <c r="A129" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B129" s="10"/>
-      <c r="C129" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D129" s="26" t="s">
+    <row r="128" spans="1:8" ht="28.8">
+      <c r="A128" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B128" s="10"/>
+      <c r="C128" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D128" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="E129" s="36"/>
-      <c r="F129" s="36"/>
-      <c r="H129" s="32"/>
+      <c r="E128" s="36"/>
+      <c r="F128" s="36"/>
+      <c r="H128" s="32"/>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D129" s="28">
+        <v>3.5</v>
+      </c>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
     </row>
     <row r="130" spans="1:8">
-      <c r="A130" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B130" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C130" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="D130" s="27">
-        <v>0.02</v>
-      </c>
+      <c r="A130" s="24"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="28"/>
+      <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
     </row>
-    <row r="131" spans="1:8">
-      <c r="B131"/>
-    </row>
-    <row r="132" spans="1:8" ht="16.8">
-      <c r="A132" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B132" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C132" s="22"/>
-      <c r="D132" s="22"/>
+    <row r="131" spans="1:8" ht="43.2">
+      <c r="A131" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B131" s="10"/>
+      <c r="C131" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D131" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E131" s="36"/>
+      <c r="F131" s="36"/>
+      <c r="H131" s="32"/>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C132" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="D132" s="28">
+        <v>6</v>
+      </c>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
     </row>
-    <row r="133" spans="1:8" s="1" customFormat="1">
-      <c r="A133" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B133" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C133" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D133" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E133" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F133" s="17"/>
-    </row>
-    <row r="134" spans="1:8" s="1" customFormat="1">
+    <row r="133" spans="1:8">
+      <c r="A133" s="24"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="28"/>
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
+    </row>
+    <row r="134" spans="1:8" ht="39" customHeight="1">
       <c r="A134" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B134" s="9"/>
+      <c r="B134" s="10"/>
       <c r="C134" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D134" s="10"/>
-      <c r="E134" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F134" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H134" t="s">
-        <v>105</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="D134" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E134" s="36"/>
+      <c r="F134" s="36"/>
+      <c r="H134" s="32"/>
     </row>
     <row r="135" spans="1:8">
-      <c r="A135" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C135" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D135" t="s">
-        <v>110</v>
-      </c>
-      <c r="E135" t="s">
-        <v>37</v>
-      </c>
-      <c r="F135">
-        <v>-30</v>
-      </c>
+      <c r="A135" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C135" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D135" s="28">
+        <v>6</v>
+      </c>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
     </row>
     <row r="136" spans="1:8">
-      <c r="B136" s="5"/>
-      <c r="D136"/>
-    </row>
-    <row r="137" spans="1:8" s="1" customFormat="1" ht="28.8">
+      <c r="A136" s="24"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="28"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+    </row>
+    <row r="137" spans="1:8" ht="28.8">
       <c r="A137" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B137" s="10"/>
       <c r="C137" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D137" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E137" s="36"/>
+      <c r="F137" s="36"/>
+      <c r="H137" s="32"/>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D138" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" s="24"/>
+      <c r="B139" s="2"/>
+      <c r="C139" s="28"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+    </row>
+    <row r="140" spans="1:8" ht="39" customHeight="1">
+      <c r="A140" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B140" s="10"/>
+      <c r="C140" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D140" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E140" s="36"/>
+      <c r="F140" s="36"/>
+      <c r="H140" s="32"/>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C141" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="D141" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" s="24"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="28"/>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+    </row>
+    <row r="143" spans="1:8" ht="43.2">
+      <c r="A143" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B143" s="10"/>
+      <c r="C143" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D143" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E143" s="36"/>
+      <c r="F143" s="36"/>
+      <c r="H143" s="32"/>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B144" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C144" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D144" s="28">
+        <v>0.06</v>
+      </c>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+    </row>
+    <row r="145" spans="1:8" ht="57.6">
+      <c r="A145" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B145" s="10"/>
+      <c r="C145" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D145" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E145" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F145" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G145" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146" t="s">
+        <v>2</v>
+      </c>
+      <c r="B146" t="s">
+        <v>12</v>
+      </c>
+      <c r="C146" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D146" t="s">
+        <v>138</v>
+      </c>
+      <c r="E146">
+        <v>0.06</v>
+      </c>
+      <c r="F146">
+        <v>45</v>
+      </c>
+      <c r="G146">
+        <v>350</v>
+      </c>
+      <c r="H146" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147" s="24"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="28"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+    </row>
+    <row r="148" spans="1:8" ht="28.8">
+      <c r="A148" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B148" s="10"/>
+      <c r="C148" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D148" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E148" s="36"/>
+      <c r="F148" s="36"/>
+      <c r="H148" s="32"/>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B149" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="D149" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" s="24"/>
+      <c r="B150" s="24"/>
+      <c r="C150" s="28"/>
+      <c r="D150" s="27"/>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+    </row>
+    <row r="151" spans="1:8" ht="57.6">
+      <c r="A151" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B151" s="10"/>
+      <c r="C151" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E151" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F151" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G151" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B152" t="s">
+        <v>12</v>
+      </c>
+      <c r="C152" t="s">
+        <v>216</v>
+      </c>
+      <c r="D152" t="s">
+        <v>138</v>
+      </c>
+      <c r="E152">
+        <v>0.04</v>
+      </c>
+      <c r="F152">
+        <v>15</v>
+      </c>
+      <c r="G152">
+        <v>150</v>
+      </c>
+      <c r="H152" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="B153"/>
+    </row>
+    <row r="154" spans="1:8" ht="16.8">
+      <c r="A154" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B154" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C154" s="22"/>
+      <c r="D154" s="22"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+    </row>
+    <row r="155" spans="1:8" s="1" customFormat="1">
+      <c r="A155" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B155" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C155" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D155" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E155" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F155" s="17"/>
+    </row>
+    <row r="156" spans="1:8" s="1" customFormat="1">
+      <c r="A156" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B156" s="9"/>
+      <c r="C156" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D156" s="10"/>
+      <c r="E156" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F156" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H156" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="A157" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D157" t="s">
+        <v>110</v>
+      </c>
+      <c r="E157" t="s">
+        <v>37</v>
+      </c>
+      <c r="F157">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="B158" s="5"/>
+      <c r="D158"/>
+    </row>
+    <row r="159" spans="1:8" s="1" customFormat="1" ht="28.8">
+      <c r="A159" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B159" s="10"/>
+      <c r="C159" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D137" s="15" t="s">
+      <c r="D159" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E137" s="29"/>
-      <c r="H137" s="4" t="s">
+      <c r="E159" s="29"/>
+      <c r="H159" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="138" spans="1:8" s="4" customFormat="1">
-      <c r="A138" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C138" s="5" t="s">
+    <row r="160" spans="1:8" s="4" customFormat="1">
+      <c r="A160" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C160" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D160" t="s">
         <v>40</v>
       </c>
-      <c r="E138"/>
-      <c r="F138"/>
-      <c r="G138"/>
-    </row>
-    <row r="139" spans="1:8" s="1" customFormat="1"/>
-    <row r="140" spans="1:8">
-      <c r="A140" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B140" s="9"/>
-      <c r="C140" s="9" t="s">
+      <c r="E160"/>
+      <c r="F160"/>
+      <c r="G160"/>
+    </row>
+    <row r="161" spans="1:6" s="1" customFormat="1"/>
+    <row r="162" spans="1:6">
+      <c r="A162" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B162" s="9"/>
+      <c r="C162" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D140" s="39" t="s">
+      <c r="D162" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="E140" s="39" t="s">
+      <c r="E162" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="F140" s="12" t="s">
+      <c r="F162" s="12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
-      <c r="A141" t="s">
-        <v>2</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C141" s="5" t="s">
+    <row r="163" spans="1:6">
+      <c r="A163" t="s">
+        <v>2</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C163" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D163" t="s">
         <v>153</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E163" t="s">
         <v>37</v>
       </c>
-      <c r="F141">
+      <c r="F163">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D57" r:id="rId1" location="Lookupcodesformanagementvariables-PLMA" display="code"/>
+    <hyperlink ref="D60" r:id="rId1" location="Lookupcodesformanagementvariables-PLMA" display="code"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>